<commit_message>
Reformatted all the Gemeinderatswahlen & Nationalratswahlen - Oberösterreich and Niederösterreich is still to do.
NÖ & OÖ still missing for both elections.
</commit_message>
<xml_diff>
--- a/Gemeinderatswahlen/csv/SALZBURG_BEREINIGT_FERTIG.xlsx
+++ b/Gemeinderatswahlen/csv/SALZBURG_BEREINIGT_FERTIG.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielkoller/Downloads/Gemeinderatswahlen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielkoller/Downloads/geowahl/Gemeinderatswahlen/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16040" yWindow="580" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="580" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -744,7 +744,7 @@
   <dimension ref="A1:F120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,6 +788,7 @@
       <c r="E2" s="3">
         <v>7259</v>
       </c>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -803,6 +804,7 @@
         <v>2081</v>
       </c>
       <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -818,6 +820,7 @@
         <v>1498</v>
       </c>
       <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -833,6 +836,7 @@
         <v>680</v>
       </c>
       <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -848,6 +852,7 @@
         <v>1281</v>
       </c>
       <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -865,6 +870,7 @@
       <c r="E7" s="3">
         <v>789</v>
       </c>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -880,6 +886,7 @@
         <v>441</v>
       </c>
       <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -897,6 +904,7 @@
       <c r="E9" s="3">
         <v>861</v>
       </c>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -914,6 +922,7 @@
       <c r="E10" s="3">
         <v>336</v>
       </c>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -931,6 +940,7 @@
       <c r="E11" s="3">
         <v>291</v>
       </c>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -946,6 +956,7 @@
         <v>319</v>
       </c>
       <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -961,6 +972,7 @@
         <v>757</v>
       </c>
       <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -976,6 +988,7 @@
         <v>534</v>
       </c>
       <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -991,6 +1004,7 @@
         <v>624</v>
       </c>
       <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1008,8 +1022,9 @@
       <c r="E16" s="3">
         <v>235</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1025,8 +1040,9 @@
       <c r="E17" s="3">
         <v>293</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1042,8 +1058,9 @@
       <c r="E18" s="3">
         <v>261</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1057,8 +1074,9 @@
         <v>571</v>
       </c>
       <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1074,8 +1092,9 @@
       <c r="E20" s="3">
         <v>286</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1087,8 +1106,9 @@
         <v>528</v>
       </c>
       <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1104,8 +1124,9 @@
       <c r="E22" s="3">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1119,8 +1140,9 @@
         <v>816</v>
       </c>
       <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1136,8 +1158,9 @@
       <c r="E24" s="3">
         <v>416</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1153,8 +1176,9 @@
       <c r="E25" s="3">
         <v>542</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1168,8 +1192,9 @@
         <v>926</v>
       </c>
       <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -1185,8 +1210,9 @@
       <c r="E27" s="3">
         <v>165</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1198,8 +1224,9 @@
         <v>364</v>
       </c>
       <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -1215,8 +1242,9 @@
       <c r="E29" s="3">
         <v>330</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1232,8 +1260,9 @@
       <c r="E30" s="3">
         <v>237</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1249,8 +1278,9 @@
       <c r="E31" s="3">
         <v>294</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -1266,8 +1296,9 @@
       <c r="E32" s="3">
         <v>283</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1281,8 +1312,9 @@
         <v>192</v>
       </c>
       <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1296,8 +1328,9 @@
         <v>974</v>
       </c>
       <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1311,8 +1344,9 @@
         <v>958</v>
       </c>
       <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1328,8 +1362,9 @@
       <c r="E36" s="3">
         <v>365</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1341,8 +1376,9 @@
         <v>804</v>
       </c>
       <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1358,8 +1394,9 @@
       <c r="E38" s="3">
         <v>258</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1375,8 +1412,9 @@
       <c r="E39" s="3">
         <v>238</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1390,8 +1428,9 @@
         <v>742</v>
       </c>
       <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>45</v>
       </c>
@@ -1407,8 +1446,9 @@
       <c r="E41" s="3">
         <v>297</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
@@ -1424,8 +1464,9 @@
       <c r="E42" s="3">
         <v>183</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>47</v>
       </c>
@@ -1439,8 +1480,9 @@
         <v>531</v>
       </c>
       <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
@@ -1454,8 +1496,9 @@
         <v>932</v>
       </c>
       <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
@@ -1469,8 +1512,9 @@
         <v>1315</v>
       </c>
       <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>50</v>
       </c>
@@ -1484,8 +1528,9 @@
         <v>320</v>
       </c>
       <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -1501,8 +1546,9 @@
       <c r="E47" s="3">
         <v>111</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
@@ -1518,8 +1564,9 @@
       <c r="E48" s="3">
         <v>259</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -1535,8 +1582,9 @@
       <c r="E49" s="3">
         <v>285</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -1552,8 +1600,9 @@
       <c r="E50" s="3">
         <v>746</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -1569,8 +1618,9 @@
       <c r="E51" s="3">
         <v>800</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
@@ -1586,8 +1636,9 @@
       <c r="E52" s="3">
         <v>1233</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -1601,8 +1652,9 @@
         <v>982</v>
       </c>
       <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>58</v>
       </c>
@@ -1616,8 +1668,9 @@
         <v>1876</v>
       </c>
       <c r="E54" s="3"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>59</v>
       </c>
@@ -1631,8 +1684,9 @@
         <v>1247</v>
       </c>
       <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
@@ -1646,8 +1700,9 @@
         <v>1744</v>
       </c>
       <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>61</v>
       </c>
@@ -1661,8 +1716,9 @@
         <v>427</v>
       </c>
       <c r="E57" s="3"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>62</v>
       </c>
@@ -1676,8 +1732,9 @@
         <v>770</v>
       </c>
       <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>63</v>
       </c>
@@ -1691,8 +1748,9 @@
         <v>511</v>
       </c>
       <c r="E59" s="3"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>64</v>
       </c>
@@ -1706,8 +1764,9 @@
         <v>937</v>
       </c>
       <c r="E60" s="3"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>65</v>
       </c>
@@ -1721,8 +1780,9 @@
         <v>173</v>
       </c>
       <c r="E61" s="3"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>66</v>
       </c>
@@ -1738,8 +1798,9 @@
       <c r="E62" s="3">
         <v>251</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>67</v>
       </c>
@@ -1751,8 +1812,9 @@
         <v>1382</v>
       </c>
       <c r="E63" s="3"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>68</v>
       </c>
@@ -1764,8 +1826,9 @@
         <v>572</v>
       </c>
       <c r="E64" s="3"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>69</v>
       </c>
@@ -1777,8 +1840,9 @@
         <v>353</v>
       </c>
       <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>70</v>
       </c>
@@ -1790,8 +1854,9 @@
         <v>269</v>
       </c>
       <c r="E66" s="3"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>71</v>
       </c>
@@ -1805,8 +1870,9 @@
         <v>315</v>
       </c>
       <c r="E67" s="3"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>72</v>
       </c>
@@ -1818,8 +1884,9 @@
         <v>1003</v>
       </c>
       <c r="E68" s="3"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>73</v>
       </c>
@@ -1833,8 +1900,9 @@
         <v>1172</v>
       </c>
       <c r="E69" s="3"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>74</v>
       </c>
@@ -1850,8 +1918,9 @@
       <c r="E70" s="3">
         <v>573</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>75</v>
       </c>
@@ -1865,8 +1934,9 @@
         <v>553</v>
       </c>
       <c r="E71" s="3"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>76</v>
       </c>
@@ -1880,8 +1950,9 @@
         <v>1183</v>
       </c>
       <c r="E72" s="3"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>77</v>
       </c>
@@ -1895,8 +1966,9 @@
         <v>253</v>
       </c>
       <c r="E73" s="3"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>78</v>
       </c>
@@ -1910,8 +1982,9 @@
         <v>101</v>
       </c>
       <c r="E74" s="3"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>79</v>
       </c>
@@ -1925,8 +1998,9 @@
         <v>793</v>
       </c>
       <c r="E75" s="3"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>80</v>
       </c>
@@ -1940,8 +2014,9 @@
         <v>765</v>
       </c>
       <c r="E76" s="3"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>81</v>
       </c>
@@ -1953,8 +2028,9 @@
         <v>247</v>
       </c>
       <c r="E77" s="3"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>82</v>
       </c>
@@ -1968,8 +2044,9 @@
         <v>132</v>
       </c>
       <c r="E78" s="3"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>83</v>
       </c>
@@ -1983,8 +2060,9 @@
         <v>217</v>
       </c>
       <c r="E79" s="3"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" s="3"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>84</v>
       </c>
@@ -1998,8 +2076,9 @@
         <v>581</v>
       </c>
       <c r="E80" s="3"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" s="3"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>85</v>
       </c>
@@ -2013,8 +2092,9 @@
         <v>663</v>
       </c>
       <c r="E81" s="3"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>86</v>
       </c>
@@ -2028,8 +2108,9 @@
         <v>178</v>
       </c>
       <c r="E82" s="3"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>87</v>
       </c>
@@ -2043,8 +2124,9 @@
         <v>369</v>
       </c>
       <c r="E83" s="3"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>88</v>
       </c>
@@ -2058,8 +2140,9 @@
         <v>242</v>
       </c>
       <c r="E84" s="3"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84" s="3"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>89</v>
       </c>
@@ -2073,8 +2156,9 @@
         <v>205</v>
       </c>
       <c r="E85" s="3"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85" s="3"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>90</v>
       </c>
@@ -2088,8 +2172,9 @@
         <v>1444</v>
       </c>
       <c r="E86" s="3"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86" s="3"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>91</v>
       </c>
@@ -2105,8 +2190,9 @@
       <c r="E87" s="3">
         <v>264</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87" s="3"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>92</v>
       </c>
@@ -2116,8 +2202,9 @@
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88" s="3"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>93</v>
       </c>
@@ -2131,8 +2218,9 @@
         <v>117</v>
       </c>
       <c r="E89" s="3"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89" s="3"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>94</v>
       </c>
@@ -2146,8 +2234,9 @@
         <v>388</v>
       </c>
       <c r="E90" s="3"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90" s="3"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>95</v>
       </c>
@@ -2161,8 +2250,9 @@
         <v>80</v>
       </c>
       <c r="E91" s="3"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91" s="3"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>96</v>
       </c>
@@ -2176,8 +2266,9 @@
         <v>489</v>
       </c>
       <c r="E92" s="3"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92" s="3"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>97</v>
       </c>
@@ -2189,8 +2280,9 @@
         <v>1354</v>
       </c>
       <c r="E93" s="3"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93" s="3"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>98</v>
       </c>
@@ -2206,8 +2298,9 @@
       <c r="E94" s="3">
         <v>265</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94" s="3"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>99</v>
       </c>
@@ -2221,8 +2314,9 @@
         <v>188</v>
       </c>
       <c r="E95" s="3"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95" s="3"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>100</v>
       </c>
@@ -2236,8 +2330,9 @@
         <v>250</v>
       </c>
       <c r="E96" s="3"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96" s="3"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>101</v>
       </c>
@@ -2251,8 +2346,9 @@
         <v>389</v>
       </c>
       <c r="E97" s="3"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97" s="3"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>102</v>
       </c>
@@ -2268,8 +2364,9 @@
       <c r="E98" s="3">
         <v>209</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98" s="3"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>103</v>
       </c>
@@ -2281,8 +2378,9 @@
         <v>286</v>
       </c>
       <c r="E99" s="3"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>104</v>
       </c>
@@ -2294,8 +2392,9 @@
         <v>425</v>
       </c>
       <c r="E100" s="3"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>105</v>
       </c>
@@ -2309,8 +2408,9 @@
         <v>1168</v>
       </c>
       <c r="E101" s="3"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>106</v>
       </c>
@@ -2324,8 +2424,9 @@
         <v>655</v>
       </c>
       <c r="E102" s="3"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>107</v>
       </c>
@@ -2339,8 +2440,9 @@
         <v>1146</v>
       </c>
       <c r="E103" s="3"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103" s="3"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>108</v>
       </c>
@@ -2354,8 +2456,9 @@
         <v>318</v>
       </c>
       <c r="E104" s="3"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104" s="3"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>109</v>
       </c>
@@ -2367,8 +2470,9 @@
       <c r="E105" s="3">
         <v>208</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105" s="3"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>110</v>
       </c>
@@ -2382,8 +2486,9 @@
         <v>583</v>
       </c>
       <c r="E106" s="3"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106" s="3"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>111</v>
       </c>
@@ -2397,8 +2502,9 @@
         <v>816</v>
       </c>
       <c r="E107" s="3"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107" s="3"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>112</v>
       </c>
@@ -2412,8 +2518,9 @@
         <v>995</v>
       </c>
       <c r="E108" s="3"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108" s="3"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>113</v>
       </c>
@@ -2425,8 +2532,9 @@
         <v>832</v>
       </c>
       <c r="E109" s="3"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109" s="3"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>114</v>
       </c>
@@ -2440,8 +2548,9 @@
         <v>775</v>
       </c>
       <c r="E110" s="3"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F110" s="3"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>115</v>
       </c>
@@ -2457,8 +2566,9 @@
       <c r="E111" s="3">
         <v>898</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F111" s="3"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>116</v>
       </c>
@@ -2474,8 +2584,9 @@
       <c r="E112" s="3">
         <v>67</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F112" s="3"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>117</v>
       </c>
@@ -2489,8 +2600,9 @@
         <v>459</v>
       </c>
       <c r="E113" s="3"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F113" s="3"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>118</v>
       </c>
@@ -2504,8 +2616,9 @@
         <v>814</v>
       </c>
       <c r="E114" s="3"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F114" s="3"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>119</v>
       </c>
@@ -2519,8 +2632,9 @@
         <v>432</v>
       </c>
       <c r="E115" s="3"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F115" s="3"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>120</v>
       </c>
@@ -2534,8 +2648,9 @@
         <v>475</v>
       </c>
       <c r="E116" s="3"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F116" s="3"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>121</v>
       </c>
@@ -2549,8 +2664,9 @@
         <v>208</v>
       </c>
       <c r="E117" s="3"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F117" s="3"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>122</v>
       </c>
@@ -2564,8 +2680,9 @@
         <v>487</v>
       </c>
       <c r="E118" s="3"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F118" s="3"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>123</v>
       </c>
@@ -2579,8 +2696,9 @@
         <v>166</v>
       </c>
       <c r="E119" s="3"/>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F119" s="3"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>124</v>
       </c>
@@ -2596,6 +2714,7 @@
       <c r="E120" s="3">
         <v>426</v>
       </c>
+      <c r="F120" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>